<commit_message>
Moved stuff around, autatic detection of controller in menu
</commit_message>
<xml_diff>
--- a/Bug Docs/GameplayBugs.xlsx
+++ b/Bug Docs/GameplayBugs.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Gameplay" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>Header</t>
   </si>
@@ -58,12 +58,18 @@
   </si>
   <si>
     <t>Sliding in die animation when killed in air or with knockback</t>
+  </si>
+  <si>
+    <t>Alchemists Graphic Pivots are off -&gt; looks weird in champion select</t>
+  </si>
+  <si>
+    <t>Active</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -89,7 +95,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -97,13 +103,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -383,16 +399,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -408,7 +424,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
@@ -419,7 +435,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -430,7 +446,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
@@ -441,7 +457,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
@@ -452,7 +468,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
@@ -463,7 +479,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
@@ -474,18 +490,29 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Bugs to doc
</commit_message>
<xml_diff>
--- a/Bug Docs/GameplayBugs.xlsx
+++ b/Bug Docs/GameplayBugs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Gameplay" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Header</t>
   </si>
@@ -64,6 +64,30 @@
   </si>
   <si>
     <t>Active</t>
+  </si>
+  <si>
+    <t>Knight Skill 4 Spear too high+</t>
+  </si>
+  <si>
+    <t>Knight attack speed too fast</t>
+  </si>
+  <si>
+    <t>Infantry Skill 1 Hook exception</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fall through not working with controller </t>
+  </si>
+  <si>
+    <t>Fall through causes stick in ground controller</t>
+  </si>
+  <si>
+    <t>Champion Selection: when 3 players, player 1 and 3 target same preview platform</t>
+  </si>
+  <si>
+    <t>Wrong team shown as winning</t>
+  </si>
+  <si>
+    <t>Running continues after game ended</t>
   </si>
 </sst>
 </file>
@@ -400,19 +424,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -423,7 +447,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -434,7 +458,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -445,7 +469,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -456,7 +480,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -467,7 +491,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -478,7 +502,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -489,7 +513,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -500,7 +524,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -509,6 +533,46 @@
       </c>
       <c r="C9" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed height of knights hook to hit all enemys
</commit_message>
<xml_diff>
--- a/Bug Docs/GameplayBugs.xlsx
+++ b/Bug Docs/GameplayBugs.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EB7F5F-A8DB-4DB3-BABE-C963453583F8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gameplay" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Header</t>
   </si>
@@ -60,15 +61,9 @@
     <t>Sliding in die animation when killed in air or with knockback</t>
   </si>
   <si>
-    <t>Alchemists Graphic Pivots are off -&gt; looks weird in champion select</t>
-  </si>
-  <si>
     <t>Active</t>
   </si>
   <si>
-    <t>Knight Skill 4 Spear too high+</t>
-  </si>
-  <si>
     <t>Knight attack speed too fast</t>
   </si>
   <si>
@@ -88,12 +83,21 @@
   </si>
   <si>
     <t>Running continues after game ended</t>
+  </si>
+  <si>
+    <t>Knight Skill 4 Spear too high</t>
+  </si>
+  <si>
+    <t>Alchemists Graphic Pivots are off -&gt; looks weird in champion select --&gt; UI Problem</t>
+  </si>
+  <si>
+    <t>Jan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -423,20 +427,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="74.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,7 +451,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -458,7 +462,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -469,7 +473,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -480,7 +484,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -491,7 +495,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -502,7 +506,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -513,7 +517,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -524,55 +528,73 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UserInput get now disabled correctly after game finished
</commit_message>
<xml_diff>
--- a/Bug Docs/GameplayBugs.xlsx
+++ b/Bug Docs/GameplayBugs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EB7F5F-A8DB-4DB3-BABE-C963453583F8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771A0153-4B9B-470B-8BED-B83C8E10A6DD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>Header</t>
   </si>
@@ -431,7 +431,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,9 +592,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed issue that alchi didn't teleport correctly through "FallThrough-Platform"
</commit_message>
<xml_diff>
--- a/Bug Docs/GameplayBugs.xlsx
+++ b/Bug Docs/GameplayBugs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF848E09-FC3D-4D09-B3DC-7917FE6ACB57}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764E3940-F2B5-47F9-9AB2-21E401FF1621}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
   <si>
     <t>Header</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>Jan</t>
+  </si>
+  <si>
+    <t>Alchi teleport ignores fallthrough-platforms</t>
   </si>
 </sst>
 </file>
@@ -144,10 +147,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -428,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,6 +619,17 @@
         <v>11</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>